<commit_message>
Re-organised the data on the Phase 1 result.
Organised the data collected from the simulation using FEMM.
</commit_message>
<xml_diff>
--- a/Phase1-Development-of-Probe/EE310-Team16-Phase1Result.xlsx
+++ b/Phase1-Development-of-Probe/EE310-Team16-Phase1Result.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/hwat294_uoa_auckland_ac_nz/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldon\Documents\ee310-team16\Phase1-Development-of-Probe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{35072492-F19A-4DF1-BF98-E22A564D12ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA9AFEED-82B5-4A3C-8A1E-D2AED7CE5F30}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12607A06-FAD6-48F8-B22A-B1ED0D41D018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38FA3C02-0BBE-4D30-BBEA-22348EE87BF5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>FEMM Simulation</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Medium</t>
-  </si>
-  <si>
-    <t>Depth</t>
   </si>
   <si>
     <t>Charge</t>
@@ -66,30 +63,6 @@
   </si>
   <si>
     <t>Water</t>
-  </si>
-  <si>
-    <t>3500mm</t>
-  </si>
-  <si>
-    <t>0mm</t>
-  </si>
-  <si>
-    <t>500mm</t>
-  </si>
-  <si>
-    <t>3000mm</t>
-  </si>
-  <si>
-    <t>2250mm</t>
-  </si>
-  <si>
-    <t>1250mm</t>
-  </si>
-  <si>
-    <t>2500mm</t>
-  </si>
-  <si>
-    <t>1000mm</t>
   </si>
   <si>
     <t>Silicone Rubber</t>
@@ -125,10 +98,25 @@
     <t>Easy, rigid</t>
   </si>
   <si>
-    <t>Cap total</t>
+    <t>Polyvinyl Chloride (PVC)</t>
   </si>
   <si>
-    <t>Polyvinyl Chloride (PVC)</t>
+    <t>Cap.Total</t>
+  </si>
+  <si>
+    <t>0% Water</t>
+  </si>
+  <si>
+    <t>20% Water</t>
+  </si>
+  <si>
+    <t>50% Water</t>
+  </si>
+  <si>
+    <t>100% Water</t>
+  </si>
+  <si>
+    <t>Depth (mm)</t>
   </si>
 </sst>
 </file>
@@ -215,26 +203,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +580,485 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-HK"/>
+              <a:t>Capacitance</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-HK" baseline="0"/>
+              <a:t> of Dielectric Material vs Change in Water Level</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-HK"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14146522309711287"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Silicone Rubber</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$22:$K$25</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0% Water</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20% Water</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50% Water</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100% Water</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$22:$L$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.4203900000000002E-11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4235454999999996E-11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.2033300000000009E-11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.398807E-10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E0BD-422D-8129-BC44A1D6DC02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Polyvinyl Chloride (PVC)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$22:$K$25</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0% Water</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20% Water</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50% Water</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100% Water</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$22:$M$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6.4987E-11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.20199E-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0301690000000001E-10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4104725000000003E-10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E0BD-422D-8129-BC44A1D6DC02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="631678768"/>
+        <c:axId val="631687888"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="631678768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="631687888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="631687888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="631678768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1145,6 +1614,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1178,6 +2163,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CDD006F-B20E-B82A-0EF0-0FC0C8A14E2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1503,10 +2524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1A8FE3-001C-405F-9F32-37A2E8D43F90}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="I9" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1529,134 +2550,134 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="5"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="9"/>
+        <v>9</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
       <c r="I5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="9"/>
+        <v>10</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="10"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="C6" s="5">
+        <v>3500</v>
       </c>
       <c r="D6">
         <f>8.84015*10^(-11)</f>
         <v>8.8401499999999987E-11</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="6">
         <v>8.8407800000000005E-11</v>
       </c>
       <c r="F6">
         <f>D6/2</f>
         <v>4.4200749999999993E-11</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="6">
         <f>E6/2</f>
         <v>4.4203900000000002E-11</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="7">
         <f>$G$6+$G$7</f>
         <v>4.4203900000000002E-11</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="6">
         <v>1.29968E-10</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="6">
         <v>1.29974E-10</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="6">
         <f>I6/2</f>
         <v>6.4984E-11</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="6">
         <f>J6/2</f>
         <v>6.4987E-11</v>
       </c>
-      <c r="M6" s="11">
-        <f>L6+L7</f>
+      <c r="M6" s="7">
+        <f>$L$6+$L$7</f>
         <v>6.4987E-11</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1668,11 +2689,11 @@
         <f t="shared" ref="F7:F13" si="0">D7/2</f>
         <v>0</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="6">
         <f t="shared" ref="G7:G13" si="1">E7/2</f>
         <v>0</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="5"/>
       <c r="I7">
         <v>0</v>
       </c>
@@ -1683,378 +2704,417 @@
         <f t="shared" ref="K7:K13" si="2">I7/2</f>
         <v>0</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="6">
         <f t="shared" ref="L7:L13" si="3">J7/2</f>
         <v>0</v>
       </c>
-      <c r="M7" s="6"/>
+      <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>0.2</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="C8" s="5">
+        <v>3000</v>
       </c>
       <c r="D8">
         <f>0.00000000007757727</f>
         <v>7.7577270000000006E-11</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="6">
         <v>7.7577809999999995E-11</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>3.8788635000000003E-11</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="6">
         <f t="shared" si="1"/>
         <v>3.8788904999999997E-11</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="7">
         <f>$G$8+$G$9</f>
         <v>6.4235454999999996E-11</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="6">
         <v>1.1140100000000001E-10</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="6">
         <v>1.11406E-10</v>
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
         <v>5.5700500000000003E-11</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="6">
         <f t="shared" si="3"/>
         <v>5.5702999999999999E-11</v>
       </c>
-      <c r="M8" s="11">
-        <f t="shared" ref="M8" si="4">L8+L9</f>
+      <c r="M8" s="7">
+        <f>$L$8+$L$9</f>
         <v>1.20199E-10</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="10">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5">
+        <v>500</v>
+      </c>
+      <c r="D9" s="6">
         <v>5.0893199999999997E-11</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="6">
         <v>5.0893099999999998E-11</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>2.5446599999999999E-11</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="6">
         <f t="shared" si="1"/>
         <v>2.5446549999999999E-11</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="10">
+      <c r="H9" s="5"/>
+      <c r="I9" s="6">
         <v>1.28992E-10</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="6">
         <v>1.28992E-10</v>
       </c>
       <c r="K9">
         <f t="shared" si="2"/>
         <v>6.4496000000000001E-11</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="6">
         <f t="shared" si="3"/>
         <v>6.4496000000000001E-11</v>
       </c>
-      <c r="M9" s="6"/>
+      <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>0.5</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="10">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2250</v>
+      </c>
+      <c r="D10" s="6">
         <v>5.6829500000000001E-11</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="6">
         <v>5.6833600000000003E-11</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
         <v>2.8414750000000001E-11</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="6">
         <f t="shared" si="1"/>
         <v>2.8416800000000001E-11</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="7">
         <f>$G$10+$G$11</f>
         <v>9.2033300000000009E-11</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="6">
         <v>8.3550599999999996E-11</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="6">
         <v>8.3554800000000003E-11</v>
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
         <v>4.1775299999999998E-11</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="6">
         <f t="shared" si="3"/>
         <v>4.1777400000000002E-11</v>
       </c>
-      <c r="M10" s="11">
-        <f t="shared" ref="M10" si="5">L10+L11</f>
+      <c r="M10" s="7">
+        <f>$L$10+$L$11</f>
         <v>2.0301690000000001E-10</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="10">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1250</v>
+      </c>
+      <c r="D11" s="6">
         <v>1.2723300000000001E-10</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="6">
         <v>1.2723300000000001E-10</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
         <v>6.3616500000000005E-11</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="6">
         <f t="shared" si="1"/>
         <v>6.3616500000000005E-11</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="10">
+      <c r="H11" s="5"/>
+      <c r="I11" s="6">
         <v>3.2248000000000001E-10</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="6">
         <v>3.22479E-10</v>
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
         <v>1.6124E-10</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="6">
         <f t="shared" si="3"/>
         <v>1.612395E-10</v>
       </c>
-      <c r="M11" s="6"/>
+      <c r="M11" s="5"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="10">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D12" s="6">
         <v>2.5257599999999999E-11</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="6">
         <v>2.52954E-11</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
         <v>1.26288E-11</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="6">
         <f t="shared" si="1"/>
         <v>1.26477E-11</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="7">
         <f>$G$12+$G$13</f>
         <v>1.398807E-10</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="6">
         <v>3.7133600000000002E-11</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="6">
         <v>3.7135500000000001E-11</v>
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
         <v>1.8566800000000001E-11</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="6">
         <f t="shared" si="3"/>
         <v>1.856775E-11</v>
       </c>
-      <c r="M12" s="11">
-        <f t="shared" ref="M12" si="6">L12+L13</f>
+      <c r="M12" s="7">
+        <f>$L$12+$L$13</f>
         <v>3.4104725000000003E-10</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="10">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5">
+        <v>2500</v>
+      </c>
+      <c r="D13" s="6">
         <v>2.5446600000000002E-10</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="6">
         <v>2.5446600000000002E-10</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
         <v>1.2723300000000001E-10</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="6">
         <f t="shared" si="1"/>
         <v>1.2723300000000001E-10</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="10">
+      <c r="H13" s="5"/>
+      <c r="I13" s="6">
         <v>6.4496000000000001E-10</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="6">
         <v>6.4495900000000001E-10</v>
       </c>
       <c r="K13">
         <f t="shared" si="2"/>
         <v>3.2248000000000001E-10</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="6">
         <f t="shared" si="3"/>
         <v>3.224795E-10</v>
       </c>
-      <c r="M13" s="6"/>
+      <c r="M13" s="5"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="10">
+      <c r="B16" s="6">
         <v>4.42E-11</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="6">
         <v>6.4999999999999995E-11</v>
       </c>
-      <c r="L16" s="12"/>
+      <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="10">
+      <c r="B17" s="6">
         <v>6.4199999999999995E-11</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="6">
         <v>1.2E-10</v>
       </c>
-      <c r="L17" s="12"/>
+      <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="10">
+      <c r="B18" s="6">
         <v>9.2000000000000005E-11</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="6">
         <v>2.03E-10</v>
       </c>
-      <c r="L18" s="12"/>
+      <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="10">
+      <c r="B19" s="6">
         <v>1.4000000000000001E-10</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="6">
         <v>3.4100000000000001E-10</v>
       </c>
-      <c r="L19" s="12"/>
+      <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L20" t="s">
-        <v>18</v>
-      </c>
-      <c r="M20" t="s">
-        <v>30</v>
-      </c>
+      <c r="L20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="11"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L21" s="2" t="s">
-        <v>29</v>
+      <c r="L21" t="s">
+        <v>9</v>
       </c>
       <c r="M21" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="12">
+        <v>11</v>
+      </c>
+      <c r="K22" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="6">
         <f>$G$6+$G$7</f>
         <v>4.4203900000000002E-11</v>
+      </c>
+      <c r="M22" s="12">
+        <f>$L$6+$L$7</f>
+        <v>6.4987E-11</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" t="s">
         <v>23</v>
       </c>
-      <c r="L23" s="12">
+      <c r="L23" s="6">
         <f>$G$8+$G$9</f>
         <v>6.4235454999999996E-11</v>
+      </c>
+      <c r="M23" s="12">
+        <f>$L$8+$L$9</f>
+        <v>1.20199E-10</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" t="s">
-        <v>26</v>
-      </c>
-      <c r="L24" s="12">
-        <f t="shared" ref="L24:L25" si="7">$G$10+$G$11</f>
+      <c r="L24" s="6">
+        <f t="shared" ref="L24" si="4">$G$10+$G$11</f>
         <v>9.2033300000000009E-11</v>
+      </c>
+      <c r="M24" s="12">
+        <f t="shared" ref="M24:M25" si="5">$L$10+$L$11</f>
+        <v>2.0301690000000001E-10</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
-      </c>
-      <c r="L25" s="12">
+        <v>19</v>
+      </c>
+      <c r="K25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25" s="6">
         <f>$G$12+$G$13</f>
         <v>1.398807E-10</v>
       </c>
+      <c r="M25" s="12">
+        <f t="shared" ref="M25:M27" si="6">$L$12+$L$13</f>
+        <v>3.4104725000000003E-10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M26" s="12"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M27" s="12"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M28" s="12"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M29" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D5:H5"/>
     <mergeCell ref="I5:M5"/>
+    <mergeCell ref="L20:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2062,6 +3122,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A61E939B809A447AEA17AA9896D8A4A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b35ad1ebb2e4c9928aa05957d3271cad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="072bdc7b-df0e-485b-ac95-1d15212e3391" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6938ddcefea5422e5e6292b196bf70c" ns3:_="">
     <xsd:import namespace="072bdc7b-df0e-485b-ac95-1d15212e3391"/>
@@ -2245,22 +3320,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA45E9B0-E326-4C83-BB53-3A23AB82EBF7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="072bdc7b-df0e-485b-ac95-1d15212e3391"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A6BB644-EE61-4E75-A0BC-3B3FBED09429}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F0105CF-884F-4349-A9C8-B301AD7AE6B6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2278,30 +3362,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A6BB644-EE61-4E75-A0BC-3B3FBED09429}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA45E9B0-E326-4C83-BB53-3A23AB82EBF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="072bdc7b-df0e-485b-ac95-1d15212e3391"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d1b36e95-0d50-42e9-958f-b63fa906beaa}" enabled="0" method="" siteId="{d1b36e95-0d50-42e9-958f-b63fa906beaa}" removed="1"/>

</xml_diff>

<commit_message>
Moved the file into the folder.
</commit_message>
<xml_diff>
--- a/Phase1-Development-of-Probe/EE310-Team16-Phase1Result.xlsx
+++ b/Phase1-Development-of-Probe/EE310-Team16-Phase1Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldon\Documents\ee310-team16\Phase1-Development-of-Probe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12607A06-FAD6-48F8-B22A-B1ED0D41D018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD09041-E2F2-4A38-8626-AB9082B54773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38FA3C02-0BBE-4D30-BBEA-22348EE87BF5}"/>
   </bookViews>
@@ -244,343 +244,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$16:$B$19</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>4.42E-11</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.4199999999999995E-11</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.2000000000000005E-11</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.4000000000000001E-10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C675-4CD6-ACA2-B701F4447747}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$16:$C$19</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6.4999999999999995E-11</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.2E-10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.03E-10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.4100000000000001E-10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C675-4CD6-ACA2-B701F4447747}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="497377247"/>
-        <c:axId val="459467039"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="497377247"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="459467039"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="459467039"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="497377247"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1058,46 +721,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1614,560 +1237,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>830580</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F670D4C4-E0AC-B9CB-ECD6-0884562A5BA2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
@@ -2198,7 +1269,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2526,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1A8FE3-001C-405F-9F32-37A2E8D43F90}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I9" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2967,39 +2038,23 @@
       <c r="M13" s="5"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="6">
-        <v>4.42E-11</v>
-      </c>
-      <c r="C16" s="6">
-        <v>6.4999999999999995E-11</v>
-      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="6">
-        <v>6.4199999999999995E-11</v>
-      </c>
-      <c r="C17" s="6">
-        <v>1.2E-10</v>
-      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="6">
-        <v>9.2000000000000005E-11</v>
-      </c>
-      <c r="C18" s="6">
-        <v>2.03E-10</v>
-      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="6">
-        <v>1.4000000000000001E-10</v>
-      </c>
-      <c r="C19" s="6">
-        <v>3.4100000000000001E-10</v>
-      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added dataset and graph for more water level.
We changed to 0%, 20%, 40%, 60%, 80% and 100% water level, and plot the line graph for that dataset.
[Just for graph only, not using it actually]

Co-Authored-By: dlee886 <100990590+dlee886@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Phase1-Development-of-Probe/EE310-Team16-Phase1Result.xlsx
+++ b/Phase1-Development-of-Probe/EE310-Team16-Phase1Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldon\Documents\ee310-team16\Phase1-Development-of-Probe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD09041-E2F2-4A38-8626-AB9082B54773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2F0A89-8921-4B5E-B974-B1D1EA4F446E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38FA3C02-0BBE-4D30-BBEA-22348EE87BF5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>FEMM Simulation</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>Depth (mm)</t>
+  </si>
+  <si>
+    <t>40% Water</t>
+  </si>
+  <si>
+    <t>60% Water</t>
+  </si>
+  <si>
+    <t>80% Water</t>
   </si>
 </sst>
 </file>
@@ -203,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -224,8 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,7 +689,631 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-HK"/>
+              <a:t>Capacitance of dielectric vs Water level</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Silicone Rubber</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0% Water</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20% Water</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40% Water</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60% Water</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80% Water</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100% Water</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$32:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>44.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BDA8-43A0-861F-1CC22434741A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Polyvinyl Chloride (PVC)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0% Water</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20% Water</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40% Water</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60% Water</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80% Water</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100% Water</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$32:$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>286</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>341</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BDA8-43A0-861F-1CC22434741A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="271743472"/>
+        <c:axId val="133840512"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="271743472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-HK"/>
+                  <a:t>Water Level</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="133840512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="133840512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-HK"/>
+                  <a:t>Capacitance (pF)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="271743472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1237,6 +1869,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1270,6 +2405,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>967740</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C1DFB0A-2669-3767-3CCB-FEF07D8B02FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1595,10 +2766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1A8FE3-001C-405F-9F32-37A2E8D43F90}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1606,7 +2777,7 @@
     <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.21875" customWidth="1"/>
@@ -2085,7 +3256,7 @@
         <f>$G$6+$G$7</f>
         <v>4.4203900000000002E-11</v>
       </c>
-      <c r="M22" s="12">
+      <c r="M22" s="6">
         <f>$L$6+$L$7</f>
         <v>6.4987E-11</v>
       </c>
@@ -2107,7 +3278,7 @@
         <f>$G$8+$G$9</f>
         <v>6.4235454999999996E-11</v>
       </c>
-      <c r="M23" s="12">
+      <c r="M23" s="6">
         <f>$L$8+$L$9</f>
         <v>1.20199E-10</v>
       </c>
@@ -2129,8 +3300,8 @@
         <f t="shared" ref="L24" si="4">$G$10+$G$11</f>
         <v>9.2033300000000009E-11</v>
       </c>
-      <c r="M24" s="12">
-        <f t="shared" ref="M24:M25" si="5">$L$10+$L$11</f>
+      <c r="M24" s="6">
+        <f t="shared" ref="M24" si="5">$L$10+$L$11</f>
         <v>2.0301690000000001E-10</v>
       </c>
     </row>
@@ -2148,28 +3319,109 @@
         <f>$G$12+$G$13</f>
         <v>1.398807E-10</v>
       </c>
-      <c r="M25" s="12">
-        <f t="shared" ref="M25:M27" si="6">$L$12+$L$13</f>
+      <c r="M25" s="6">
+        <f t="shared" ref="M25" si="6">$L$12+$L$13</f>
         <v>3.4104725000000003E-10</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M26" s="12"/>
+      <c r="M26" s="6"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M27" s="12"/>
+      <c r="M27" s="6"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M28" s="12"/>
+      <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M29" s="13"/>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C30" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="11"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="12">
+        <v>44.2</v>
+      </c>
+      <c r="D32" s="12">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="12">
+        <v>64.2</v>
+      </c>
+      <c r="D33" s="12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="12">
+        <v>82.4</v>
+      </c>
+      <c r="D34" s="12">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="12">
+        <v>102</v>
+      </c>
+      <c r="D35" s="12">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="12">
+        <v>121</v>
+      </c>
+      <c r="D36" s="12">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="12">
+        <v>140</v>
+      </c>
+      <c r="D37" s="12">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D38" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="D5:H5"/>
     <mergeCell ref="I5:M5"/>
     <mergeCell ref="L20:M20"/>
+    <mergeCell ref="C30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2177,21 +3429,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A61E939B809A447AEA17AA9896D8A4A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b35ad1ebb2e4c9928aa05957d3271cad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="072bdc7b-df0e-485b-ac95-1d15212e3391" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6938ddcefea5422e5e6292b196bf70c" ns3:_="">
     <xsd:import namespace="072bdc7b-df0e-485b-ac95-1d15212e3391"/>
@@ -2375,31 +3612,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA45E9B0-E326-4C83-BB53-3A23AB82EBF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="072bdc7b-df0e-485b-ac95-1d15212e3391"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A6BB644-EE61-4E75-A0BC-3B3FBED09429}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F0105CF-884F-4349-A9C8-B301AD7AE6B6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2417,6 +3645,30 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A6BB644-EE61-4E75-A0BC-3B3FBED09429}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA45E9B0-E326-4C83-BB53-3A23AB82EBF7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="072bdc7b-df0e-485b-ac95-1d15212e3391"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d1b36e95-0d50-42e9-958f-b63fa906beaa}" enabled="0" method="" siteId="{d1b36e95-0d50-42e9-958f-b63fa906beaa}" removed="1"/>

</xml_diff>